<commit_message>
se agrego manual de usuario y lista chequeo actualizada
</commit_message>
<xml_diff>
--- a/assets/docs/trim5/PFPL01 - Lista de chequeo producto software.xlsx
+++ b/assets/docs/trim5/PFPL01 - Lista de chequeo producto software.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Desktop\mgm2\TPS_FDS_2671339_PMGM6\assets\docs\trim5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DC31AF-2137-4BA0-B79D-E72C9A1592BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="772" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <definedName name="vertex42_id" hidden="1">"gantt-chart_L.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Gantt Chart Template"</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="109">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -200,21 +199,12 @@
     <t>OTROS:</t>
   </si>
   <si>
-    <t>¿El sistema de información cuenta con componentes que actúen como “compresores”, es decir, proyectados para recibir más información de la que transmiten? (Compresión)</t>
-  </si>
-  <si>
     <t>¿Se ofrecen las herramientas necesarias para añadir, borrar, mantener, exhibir, imprimir, buscar y actualizar datos?</t>
   </si>
   <si>
-    <t>¿Se cumple con la función de procesamiento, que implica la modificación de la base de datos para mantenerla actualizada? (Procesamiento)</t>
-  </si>
-  <si>
     <t>¿Permite la recuperación de datos en tiempo real? (Recuperación)</t>
   </si>
   <si>
-    <t>¿Se han especificado las pre-condiciones para cada una de las funcionalidades del sistema/software?</t>
-  </si>
-  <si>
     <t>¿El sistema tiene configurado un tiempo máximo de sesión de usuario?</t>
   </si>
   <si>
@@ -224,15 +214,6 @@
     <t>¿Se han especificado otras consideraciones temporales, tales como el tiempo de procesamiento, el de transferencia de datos o la tasa de transferencia?</t>
   </si>
   <si>
-    <t xml:space="preserve">¿Se ha establecido el tiempo promedio de movimiento entre pantallas? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Se ha establecido, para el uso de la memoria del servidor, un porcentaje que no exceda el uso de la memoria disponible? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Se ha establecido el tiempo máximo de movimiento entre pantallas? </t>
-  </si>
-  <si>
     <t>¿Se ha especificado la fiabilidad del sistema/software, incluyendo las consecuencias en el caso de que falle?</t>
   </si>
   <si>
@@ -254,60 +235,30 @@
     <t>¿Se ha defnido cómo ser reemplazado por otro producto software teniendo en cuenta el mismo propósito y entorno del software?</t>
   </si>
   <si>
-    <t>¿Se ha definido el sistema operativo que se va a utilizar? *móvil</t>
-  </si>
-  <si>
-    <t>¿Se ha definido la versión del sistema operativo? *móvil</t>
-  </si>
-  <si>
     <t>¿Se especificaron las consecuencias por causa de fallas en la implementación del requerimiento?</t>
   </si>
   <si>
     <t>¿Se definió el plan de contingencia en caso de fallas?</t>
   </si>
   <si>
-    <t>¿Se definió la estrategia de detección y corrección de errores a causa de las fallas?</t>
-  </si>
-  <si>
-    <t>¿Se identifican en los requisitos atributos relacionados con la capacidad del sistema para mantener su nivel de prestación de servicio en las condiciones establecidas durante un período?</t>
-  </si>
-  <si>
     <t xml:space="preserve">¿La capacidad del sistema para tolerar errores está especificada en los requisitos? </t>
   </si>
   <si>
-    <t>¿La capacidad del sistema para tolerar sobrecargas en el volumen de información, de usuarios o de procesos está especifica_x0002_da en los requisitos?</t>
-  </si>
-  <si>
     <t>¿Se tiene prevista la capacidad de protección contra el acceso de datos e información no autorizados, ya sea accidental o de_x0002_liberadamente?</t>
   </si>
   <si>
     <t>¿Se considera el control de accesos o modificaciones no autorizados a datos o programas de ordenador?</t>
   </si>
   <si>
-    <t>¿Se tiene previsto demostrar la identidad de un sujeto o un recurso?</t>
-  </si>
-  <si>
-    <t>¿Se incluye la respuesta del sistema a los cambios en el entorno operativo, las interfaces, la precisión, el rendimiento, y otras capacidades adicionales predecibles?</t>
-  </si>
-  <si>
-    <t>¿Se incluye la manera en que el sistema interactuará con otros software?</t>
-  </si>
-  <si>
     <t>¿Se especifica la comunicación del sistema con otros sistemas software?</t>
   </si>
   <si>
     <t>¿Se determina cuáles son los recursos que el sistema compartirá con otros productos software y cómo se hará dicho proceso?</t>
   </si>
   <si>
-    <t>¿Se especifica el ambiente sobre el cual el sistema funcionará y con cuáles ambientes no lo hará?</t>
-  </si>
-  <si>
     <t>¿Se especifican los requerimientos software y hardware sobre los cuales el sistema funcionará correctamente?</t>
   </si>
   <si>
-    <t>¿Se especifican las conexiones soporta el sistema en un día sin reducir su rendimiento?</t>
-  </si>
-  <si>
     <t>¿Se especifican requisitos mínimos necesarios para que la aplicación funcione correctamente?</t>
   </si>
   <si>
@@ -317,66 +268,27 @@
     <t>¿Se especifica cómo interactuará el sistema con el servicio en la nube que escojan?</t>
   </si>
   <si>
-    <t>¿Se ha especificado el concepto de usabilidad para el sistema/software?</t>
-  </si>
-  <si>
-    <t>¿Se ha especificado, bajo el concepto de usabilidad, cuál será el objetivo de este dentro del sistema/software?</t>
-  </si>
-  <si>
     <t>¿Se ha especificado si existen necesidades gráficas o de interfaz particulares, en torno a usabilidad teniendo en cuenta los usuarios finales del sistema/software?</t>
   </si>
   <si>
     <t>¿Se ha especificado un panorama general respecto a la interfaz del sistema/software, como: colores, fuentes, logos?</t>
   </si>
   <si>
-    <t>¿Se ha especificado si el sistema/software debe cumplir con requerimientos de accesibilidad y/o para personas con alguna discapacidad?</t>
-  </si>
-  <si>
-    <t>¿Se ha especificado según el concepto anterior dichos requerimientos de accesibilidad?</t>
-  </si>
-  <si>
-    <t>¿Se ha especificado claramente de qué forma se accede a las funcionalidades del sistema/software</t>
-  </si>
-  <si>
     <t>¿Se han especificado los requerimientos para la comunicación entre los componentes del sistema/software?</t>
   </si>
   <si>
     <t>¿Se han definido las interfaces externas, como por ejemplo usuarios o hardware?</t>
   </si>
   <si>
-    <t>¿Se han definido las interfaces internas, como por ejemplo el software o el hardware?</t>
-  </si>
-  <si>
     <t>¿El sistema tiene la capacidad, cuando hay cambios en componentes, de que exista un impacto mínimo en los demás?</t>
   </si>
   <si>
     <t>¿El sistema permite que sus componentes sean utilizados en los demás elementos del mismo, o en la construcción de nuevos componentes? (Reusabilidad)</t>
   </si>
   <si>
-    <t>¿El sistema cuenta con facilidad en el momento de evaluar el impacto con un determinado cambio sobre el software?</t>
-  </si>
-  <si>
-    <t>¿El sistema cuenta con la capacidad de ser modificado sin introducir defectos o degradar el desempeñ</t>
-  </si>
-  <si>
     <t>¿El sistema cuenta con facilidad para establecer criterios de prueba?</t>
   </si>
   <si>
-    <t xml:space="preserve">El sistema debe pedir el inicio de sesión al usuario   </t>
-  </si>
-  <si>
-    <t>el sistema debe permitir crear nuevos usuarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema debe permitir actualizar usuarios </t>
-  </si>
-  <si>
-    <t>El sistema debería permitir eliminar usuarios</t>
-  </si>
-  <si>
-    <t>El sistema deberá permitir consultar el estado de los usuarios</t>
-  </si>
-  <si>
     <t xml:space="preserve">El sistema debe permitir crear nuevos productos </t>
   </si>
   <si>
@@ -417,13 +329,46 @@
   </si>
   <si>
     <t xml:space="preserve">El sistema debe permitir generar un reporte de ventas mensual </t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al admin y el vendedor iniciar sesión</t>
+  </si>
+  <si>
+    <t>el sistema debe permitir al admin crear nuevos usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir actualizar al admin usuarios </t>
+  </si>
+  <si>
+    <t>El sistema debería permitir al admin eliminar usuarios</t>
+  </si>
+  <si>
+    <t>El sistema deberá permitir al admin consultar el estado de los usuarios</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Proveedores</t>
+  </si>
+  <si>
+    <t>Reportes</t>
+  </si>
+  <si>
+    <t>Cumple</t>
+  </si>
+  <si>
+    <t>No Cumple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +465,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -535,7 +488,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1176,19 +1129,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1344,6 +1284,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1382,12 +1335,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1412,6 +1359,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1424,42 +1386,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2" xr:uid="{1EB9EC41-D830-4ACE-B66C-36C057A1DC02}"/>
+    <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{1BF490CB-4EC1-4FFF-9B5A-A574EBD0F1D4}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1821,115 +1761,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A635BB-A94A-407B-BBB0-F2B3339CC475}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P82"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="12" style="9" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="9" customWidth="1"/>
     <col min="4" max="4" width="28" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="35.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="26.26953125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="35.1796875" style="9" customWidth="1"/>
     <col min="7" max="8" width="12" style="9" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="16.7265625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="19.1796875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.1796875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" style="9" customWidth="1"/>
     <col min="13" max="256" width="12" style="9" customWidth="1"/>
-    <col min="257" max="257" width="12.5703125" style="9" customWidth="1"/>
-    <col min="258" max="16384" width="11.42578125" style="9"/>
+    <col min="257" max="257" width="12.54296875" style="9" customWidth="1"/>
+    <col min="258" max="16384" width="11.453125" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-    </row>
-    <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="79" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+    </row>
+    <row r="3" spans="2:6" ht="30.5">
+      <c r="B3" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-    </row>
-    <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="79" t="s">
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+    </row>
+    <row r="4" spans="2:6" ht="30.5">
+      <c r="B4" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-    </row>
-    <row r="5" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-    </row>
-    <row r="6" spans="2:6" ht="17.25" thickTop="1">
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+    </row>
+    <row r="5" spans="2:6" ht="14.5" thickBot="1">
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+    </row>
+    <row r="6" spans="2:6" ht="14.5" thickTop="1">
       <c r="F6" s="10"/>
     </row>
-    <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="81" t="s">
+    <row r="8" spans="2:6" ht="30.5">
+      <c r="B8" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-    </row>
-    <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
-    <row r="11" spans="2:6" ht="18.75" thickTop="1">
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+    </row>
+    <row r="10" spans="2:6" ht="14.5" thickBot="1"/>
+    <row r="11" spans="2:6" ht="18.5" thickTop="1">
       <c r="B11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="85"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="70"/>
-    </row>
-    <row r="13" spans="2:6" ht="18.75" thickBot="1">
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+    </row>
+    <row r="13" spans="2:6" ht="18.5" thickBot="1">
       <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="70"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="73"/>
     </row>
     <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="72"/>
+      <c r="D14" s="75"/>
       <c r="E14" s="13" t="s">
         <v>24</v>
       </c>
@@ -1941,10 +1881,10 @@
       <c r="B15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="74"/>
+      <c r="D15" s="77"/>
       <c r="E15" s="15" t="s">
         <v>28</v>
       </c>
@@ -1956,10 +1896,10 @@
       <c r="B16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="76"/>
+      <c r="D16" s="79"/>
       <c r="E16" s="17" t="s">
         <v>31</v>
       </c>
@@ -1967,10 +1907,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="17.25" thickTop="1">
+    <row r="17" spans="2:16" ht="16" thickTop="1">
       <c r="B17" s="19"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -1989,10 +1929,10 @@
       <c r="C21" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="66" t="s">
+      <c r="D21" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="66"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="24" t="s">
         <v>37</v>
       </c>
@@ -2004,10 +1944,10 @@
       <c r="C22" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="67"/>
+      <c r="E22" s="82"/>
       <c r="F22" s="27" t="s">
         <v>25</v>
       </c>
@@ -2015,57 +1955,57 @@
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
       <c r="F23" s="30"/>
     </row>
     <row r="24" spans="2:16" ht="25.5" customHeight="1">
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="2:16" ht="25.5" customHeight="1">
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:16" ht="25.5" customHeight="1">
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="2:16" ht="25.5" customHeight="1">
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="2:16" ht="25.5" customHeight="1">
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="2:16" ht="25.5" customHeight="1">
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
       <c r="F30" s="33"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -2076,51 +2016,51 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="62"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="67"/>
     </row>
     <row r="35" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="63"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="65"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="70"/>
     </row>
     <row r="36" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="52"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="54"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="59"/>
       <c r="J36" s="34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="52"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="59"/>
     </row>
     <row r="38" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="52"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="59"/>
     </row>
     <row r="39" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="62"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A40" s="34"/>
@@ -2318,26 +2258,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC27DB5-F54D-4E92-8170-7A53853F8C0C}">
-  <dimension ref="A1:D70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="70.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="70.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="70.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="43" t="s">
+        <v>103</v>
+      </c>
       <c r="C1" s="41"/>
       <c r="D1" s="42"/>
     </row>
@@ -2359,74 +2301,80 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="87" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="B3" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D3" s="6" t="str">
         <f>IF(C3="Cumple","Ninguna","")</f>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="87" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="5"/>
+      <c r="B4" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D4" s="6" t="str">
-        <f t="shared" ref="D4:D17" si="0">IF(C4="Cumple","Ninguna","")</f>
-        <v/>
+        <f t="shared" ref="D4:D10" si="0">IF(C4="Cumple","Ninguna","")</f>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="87" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="B5" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="87" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="B6" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="87" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="B7" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="87" t="s">
-        <v>113</v>
-      </c>
+      <c r="A8" s="8"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2434,12 +2382,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="8">
-        <v>7</v>
-      </c>
-      <c r="B9" s="87" t="s">
-        <v>114</v>
-      </c>
+      <c r="A9" s="8"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2447,722 +2391,442 @@
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="87" t="s">
-        <v>115</v>
-      </c>
+      <c r="A10" s="8"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="8">
-        <v>9</v>
-      </c>
-      <c r="B11" s="87" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6" t="str">
-        <f t="shared" si="0"/>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A11" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+    </row>
+    <row r="12" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A13" s="53">
+        <v>16</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="6" t="str">
+        <f t="shared" ref="D13:D20" si="1">IF(C13="Cumple","Ninguna","")</f>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A14" s="53">
+        <v>17</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6" t="str">
-        <f t="shared" si="0"/>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A15" s="53">
+        <v>18</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="6" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="8">
-        <v>11</v>
-      </c>
-      <c r="B13" s="87" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A14" s="8">
-        <v>12</v>
-      </c>
-      <c r="B14" s="87" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="8">
-        <v>13</v>
-      </c>
-      <c r="B15" s="87" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
     <row r="16" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="8">
-        <v>14</v>
-      </c>
-      <c r="B16" s="87" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="5"/>
+      <c r="A16" s="53">
+        <v>19</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>108</v>
+      </c>
       <c r="D16" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A17" s="8">
-        <v>15</v>
-      </c>
-      <c r="B17" s="87" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D17" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="90" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="88">
-        <v>16</v>
-      </c>
-      <c r="B20" s="92" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="89"/>
-      <c r="D20" s="6" t="str">
-        <f t="shared" ref="D20:D34" si="1">IF(C20="Cumple","Ninguna","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="88">
-        <v>17</v>
-      </c>
-      <c r="B21" s="92" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="89"/>
-      <c r="D21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="88">
-        <v>18</v>
-      </c>
-      <c r="B22" s="92" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="89"/>
-      <c r="D22" s="6" t="str">
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="88">
-        <v>19</v>
-      </c>
-      <c r="B23" s="92" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="89"/>
-      <c r="D23" s="6" t="str">
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
+    <row r="21" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A22" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A23" s="8">
+        <v>31</v>
+      </c>
+      <c r="B23" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f t="shared" ref="D23:D30" si="2">IF(C23="Cumple","Ninguna","")</f>
+        <v>Ninguna</v>
+      </c>
+    </row>
     <row r="24" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A24" s="8">
-        <v>20</v>
-      </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B24" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D24" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A25" s="8">
-        <v>21</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="B25" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D25" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A26" s="8">
-        <v>22</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D26" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A27" s="8">
-        <v>23</v>
-      </c>
+      <c r="A27" s="8"/>
       <c r="B27" s="6"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="8">
-        <v>24</v>
-      </c>
+      <c r="A28" s="8"/>
       <c r="B28" s="6"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="8">
-        <v>25</v>
-      </c>
+      <c r="A29" s="8"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A30" s="8">
-        <v>26</v>
-      </c>
+      <c r="A30" s="8"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A31" s="8">
-        <v>27</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A32" s="8">
-        <v>28</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+    <row r="31" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A31" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
+    </row>
+    <row r="32" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A32" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A33" s="8">
-        <v>29</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="B33" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D33" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" ref="D33:D41" si="3">IF(C33="Cumple","Ninguna","")</f>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A34" s="8">
-        <v>30</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B34" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D34" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A35" s="44" t="s">
+    <row r="35" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A35" s="8">
+        <v>48</v>
+      </c>
+      <c r="B35" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A36" s="8">
         <v>49</v>
       </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-    </row>
-    <row r="36" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A36" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>7</v>
+      <c r="B36" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A37" s="8">
-        <v>31</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="B37" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="92" t="s">
+        <v>107</v>
+      </c>
       <c r="D37" s="6" t="str">
-        <f t="shared" ref="D37:D51" si="2">IF(C37="Cumple","Ninguna","")</f>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A38" s="8">
-        <v>32</v>
-      </c>
+      <c r="A38" s="8"/>
       <c r="B38" s="6"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A39" s="8">
-        <v>33</v>
-      </c>
+      <c r="A39" s="8"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A40" s="8">
-        <v>34</v>
-      </c>
+      <c r="A40" s="8"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A41" s="8">
-        <v>35</v>
-      </c>
+      <c r="A41" s="8"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A42" s="8">
-        <v>36</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A43" s="8">
-        <v>37</v>
-      </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A44" s="8">
-        <v>38</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A45" s="8">
-        <v>39</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A46" s="8">
-        <v>40</v>
-      </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A47" s="8">
-        <v>41</v>
-      </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A48" s="8">
-        <v>42</v>
-      </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A49" s="8">
-        <v>43</v>
-      </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A50" s="8">
-        <v>44</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A51" s="8">
-        <v>45</v>
-      </c>
-      <c r="B51" s="6"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A52" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="42"/>
-    </row>
-    <row r="53" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A53" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A54" s="8">
-        <v>46</v>
-      </c>
-      <c r="B54" s="6"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6" t="str">
-        <f t="shared" ref="D54:D68" si="3">IF(C54="Cumple","Ninguna","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A55" s="8">
-        <v>47</v>
-      </c>
-      <c r="B55" s="6"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A56" s="8">
-        <v>48</v>
-      </c>
-      <c r="B56" s="6"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A57" s="8">
-        <v>49</v>
-      </c>
-      <c r="B57" s="6"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A58" s="8">
-        <v>50</v>
-      </c>
-      <c r="B58" s="6"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A59" s="8">
-        <v>51</v>
-      </c>
-      <c r="B59" s="6"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A60" s="8">
-        <v>52</v>
-      </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A61" s="8">
+    <row r="42" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A42" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A62" s="8">
-        <v>54</v>
-      </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A63" s="8">
-        <v>55</v>
-      </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A64" s="8">
-        <v>56</v>
-      </c>
-      <c r="B64" s="6"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A65" s="8">
-        <v>57</v>
-      </c>
-      <c r="B65" s="6"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A66" s="8">
-        <v>58</v>
-      </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A67" s="8">
-        <v>59</v>
-      </c>
-      <c r="B67" s="6"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A68" s="8">
-        <v>60</v>
-      </c>
-      <c r="B68" s="6"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A69" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B69" s="43"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="42"/>
-    </row>
-    <row r="70" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A70" s="45" t="s">
+      <c r="B42" s="43"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+    </row>
+    <row r="43" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A43" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="39" t="s">
+      <c r="B43" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="39" t="s">
+      <c r="C43" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="39" t="s">
+      <c r="D43" s="39" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C17 C20:C34 C37:C51 C54:C68" xr:uid="{F381E73E-C892-4E35-A1B1-7DCF65F35B27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C10 C13:C20 C23:C30 C33:C41">
       <formula1>"Cumple, No Cumple"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="90.7109375" style="51" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="90.7265625" style="51" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
@@ -3186,10 +2850,12 @@
       <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D2" s="6" t="str">
         <f>IF(C2="Cumple","Ninguna","")</f>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
@@ -3199,10 +2865,12 @@
       <c r="B3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D3" s="6" t="str">
-        <f t="shared" ref="D3:D65" si="0">IF(C3="Cumple","Ninguna","")</f>
-        <v/>
+        <f t="shared" ref="D3:D41" si="0">IF(C3="Cumple","Ninguna","")</f>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
@@ -3212,7 +2880,9 @@
       <c r="B4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3220,51 +2890,58 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="8">
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="D7" s="39" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3272,157 +2949,177 @@
     </row>
     <row r="9" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A10" s="8">
+        <v>11</v>
+      </c>
+      <c r="B10" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="str">
+      <c r="C10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="8">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B11" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+    <row r="12" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A13" s="8">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A14" s="8">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="8">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="8">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B16" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A17" s="8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B17" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="8">
+        <v>21</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6" t="str">
+      <c r="C18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="39" t="s">
+    <row r="19" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="39" t="s">
+      <c r="B19" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D19" s="39" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="8">
-        <v>16</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
       </c>
     </row>
     <row r="20" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="8">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3430,225 +3127,254 @@
     </row>
     <row r="21" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="8">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B21" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" customHeight="1">
+      <c r="A22" s="8">
+        <v>28</v>
+      </c>
+      <c r="B22" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6" t="str">
+      <c r="C22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="8">
-        <v>19</v>
-      </c>
-      <c r="B22" s="50" t="s">
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A23" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" customHeight="1">
+      <c r="A24" s="8">
+        <v>30</v>
+      </c>
+      <c r="B24" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="8">
-        <v>20</v>
-      </c>
-      <c r="B23" s="50" t="s">
+      <c r="C24" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" customHeight="1">
+      <c r="A25" s="8">
+        <v>31</v>
+      </c>
+      <c r="B25" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A24" s="8">
-        <v>21</v>
-      </c>
-      <c r="B24" s="50" t="s">
+      <c r="C25" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A26" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" customHeight="1">
+      <c r="A27" s="8">
+        <v>35</v>
+      </c>
+      <c r="B27" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A25" s="8">
-        <v>22</v>
-      </c>
-      <c r="B25" s="50" t="s">
+      <c r="C27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" customHeight="1">
+      <c r="A28" s="8">
+        <v>36</v>
+      </c>
+      <c r="B28" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A26" s="8">
-        <v>23</v>
-      </c>
-      <c r="B26" s="50" t="s">
+      <c r="C28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" customHeight="1">
+      <c r="A29" s="8">
+        <v>38</v>
+      </c>
+      <c r="B29" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A27" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="8">
-        <v>24</v>
-      </c>
-      <c r="B28" s="50" t="s">
+      <c r="C29" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" customHeight="1">
+      <c r="A30" s="8">
+        <v>40</v>
+      </c>
+      <c r="B30" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="8">
-        <v>25</v>
-      </c>
-      <c r="B29" s="50" t="s">
+      <c r="C30" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" customHeight="1">
+      <c r="A31" s="8">
+        <v>41</v>
+      </c>
+      <c r="B31" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A30" s="8">
-        <v>26</v>
-      </c>
-      <c r="B30" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A31" s="8">
-        <v>27</v>
-      </c>
-      <c r="B31" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" customHeight="1">
       <c r="A32" s="8">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" customHeight="1">
-      <c r="A33" s="8">
-        <v>29</v>
-      </c>
-      <c r="B33" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A34" s="39" t="s">
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A33" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="39" t="s">
+      <c r="B33" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D33" s="39" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" customHeight="1">
+      <c r="A34" s="8">
+        <v>45</v>
+      </c>
+      <c r="B34" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" customHeight="1">
       <c r="A35" s="8">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" customHeight="1">
       <c r="A36" s="8">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B36" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" customHeight="1">
       <c r="A37" s="8">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
@@ -3656,7 +3382,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C38" s="39" t="s">
         <v>6</v>
@@ -3667,360 +3393,52 @@
     </row>
     <row r="39" spans="1:4" ht="30" customHeight="1">
       <c r="A39" s="8">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" customHeight="1">
       <c r="A40" s="8">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" customHeight="1">
       <c r="A41" s="8">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" customHeight="1">
-      <c r="A42" s="8">
-        <v>36</v>
-      </c>
-      <c r="B42" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" customHeight="1">
-      <c r="A43" s="8">
-        <v>37</v>
-      </c>
-      <c r="B43" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" customHeight="1">
-      <c r="A44" s="8">
-        <v>38</v>
-      </c>
-      <c r="B44" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" customHeight="1">
-      <c r="A45" s="8">
-        <v>39</v>
-      </c>
-      <c r="B45" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" customHeight="1">
-      <c r="A46" s="8">
-        <v>40</v>
-      </c>
-      <c r="B46" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="30" customHeight="1">
-      <c r="A47" s="8">
-        <v>41</v>
-      </c>
-      <c r="B47" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30" customHeight="1">
-      <c r="A48" s="8">
-        <v>42</v>
-      </c>
-      <c r="B48" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A49" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1">
-      <c r="A50" s="8">
-        <v>43</v>
-      </c>
-      <c r="B50" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30" customHeight="1">
-      <c r="A51" s="8">
-        <v>44</v>
-      </c>
-      <c r="B51" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" customHeight="1">
-      <c r="A52" s="8">
-        <v>45</v>
-      </c>
-      <c r="B52" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30" customHeight="1">
-      <c r="A53" s="8">
-        <v>46</v>
-      </c>
-      <c r="B53" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30" customHeight="1">
-      <c r="A54" s="8">
-        <v>47</v>
-      </c>
-      <c r="B54" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="30" customHeight="1">
-      <c r="A55" s="8">
-        <v>48</v>
-      </c>
-      <c r="B55" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="30" customHeight="1">
-      <c r="A56" s="8">
-        <v>49</v>
-      </c>
-      <c r="B56" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="30" customHeight="1">
-      <c r="A57" s="8">
-        <v>50</v>
-      </c>
-      <c r="B57" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30" customHeight="1">
-      <c r="A58" s="8">
-        <v>51</v>
-      </c>
-      <c r="B58" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30" customHeight="1">
-      <c r="A59" s="8">
-        <v>52</v>
-      </c>
-      <c r="B59" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A60" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30" customHeight="1">
-      <c r="A61" s="8">
-        <v>53</v>
-      </c>
-      <c r="B61" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30" customHeight="1">
-      <c r="A62" s="8">
-        <v>54</v>
-      </c>
-      <c r="B62" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="30" customHeight="1">
-      <c r="A63" s="8">
-        <v>55</v>
-      </c>
-      <c r="B63" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="30" customHeight="1">
-      <c r="A64" s="8">
-        <v>56</v>
-      </c>
-      <c r="B64" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="30" customHeight="1">
-      <c r="A65" s="8">
-        <v>57</v>
-      </c>
-      <c r="B65" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9 C11:C17 C19:C26 C28:C32 C50:C59 C39:C48 C33 C35:C37" xr:uid="{28946FFD-2DE3-4AFF-8B02-311FA9F788A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C18 C24:C25 C8:C11 C2:C6 C27:C32 C34:C37 C20:C22">
       <formula1>"Cumple, No Cumple"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4029,17 +3447,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D51D51-DE4C-4B5C-90F6-8EADB68EB458}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1">
@@ -4058,7 +3478,7 @@
       <c r="E1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="90" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4071,17 +3491,17 @@
       </c>
       <c r="C2" s="5">
         <f>COUNT('Requisitos Funcionales'!A:A)</f>
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5">
-        <f>COUNTIF('Requisitos Funcionales'!C2:C68,"Cumple")</f>
-        <v>0</v>
+        <f>COUNTIF('Requisitos Funcionales'!C2:C41,"Cumple")</f>
+        <v>13</v>
       </c>
       <c r="E2" s="48">
         <f>D2/C2%</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="86"/>
+        <v>68.421052631578945</v>
+      </c>
+      <c r="F2" s="91"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1">
       <c r="A3" s="47">
@@ -4092,34 +3512,34 @@
       </c>
       <c r="C3" s="5">
         <f>COUNT('Requisitos No Funcionales'!A:A)</f>
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5">
         <f>COUNTIF('Requisitos No Funcionales'!C:C,"Cumple")</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E3" s="48">
         <f t="shared" ref="E3:E4" si="0">D3/C3%</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="86"/>
+        <v>75.757575757575751</v>
+      </c>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
       <c r="C4" s="46">
         <f>SUM(C2:C3)</f>
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="D4" s="46">
         <f>SUM(D2:D3)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E4" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>73.07692307692308</v>
       </c>
       <c r="F4" s="5" t="str">
         <f>IF(E4&gt;=90,"APROBADO",IF(AND(E4&gt;=70,E4&lt;90),"CORREGIR","NO APROBADO"))</f>
-        <v>NO APROBADO</v>
+        <v>CORREGIR</v>
       </c>
     </row>
   </sheetData>

</xml_diff>